<commit_message>
Recorded and Finished several sounds
Recorded voiceover sounds and fixed them up in Reaper (robotic, radio calls, etcetera)
</commit_message>
<xml_diff>
--- a/DOCUMENTATION/Sound Asset List.xlsx
+++ b/DOCUMENTATION/Sound Asset List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity\Unity Projects\SpacemanLandF\DOCUMENTATION\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10197FA3-BA53-49F3-8409-CCA4072B9331}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E61F195D-1D66-4950-89AA-32F35737BC52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="75">
   <si>
     <t>Dialog</t>
   </si>
@@ -347,6 +347,9 @@
   </si>
   <si>
     <t>In-Game (work needed)</t>
+  </si>
+  <si>
+    <t>Reaper Done</t>
   </si>
 </sst>
 </file>
@@ -508,7 +511,7 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1">
       <alignment horizontal="center"/>
@@ -526,13 +529,14 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="6" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="2" xfId="8" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="4" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="5" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="6" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="8" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="2" xfId="8" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="5" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="40% - Accent1" xfId="4" builtinId="31"/>
@@ -824,7 +828,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -913,8 +917,8 @@
       <c r="E4" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="6" t="s">
-        <v>64</v>
+      <c r="F4" s="16" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -953,7 +957,7 @@
       <c r="E6" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="F6" s="9" t="s">
         <v>72</v>
       </c>
     </row>
@@ -973,7 +977,7 @@
       <c r="E7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="9" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1073,7 +1077,7 @@
       <c r="E12" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="F12" s="15" t="s">
+      <c r="F12" s="9" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1103,49 +1107,49 @@
       </c>
     </row>
     <row r="17" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D17" s="9" t="s">
+      <c r="D17" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
     </row>
     <row r="19" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C19" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="D19" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
     </row>
     <row r="20" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D20" s="12" t="s">
+      <c r="D20" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
     </row>
     <row r="21" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D21" s="14" t="s">
+      <c r="D21" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
     </row>
     <row r="22" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D22" s="13" t="s">
+      <c r="D22" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
small Sound Asset List Update
</commit_message>
<xml_diff>
--- a/DOCUMENTATION/Sound Asset List.xlsx
+++ b/DOCUMENTATION/Sound Asset List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity\Unity Projects\SpacemanLandF\DOCUMENTATION\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E61F195D-1D66-4950-89AA-32F35737BC52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCCDD3DC-36EB-48B6-8591-3C2B89A40442}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="74">
   <si>
     <t>Dialog</t>
   </si>
@@ -219,33 +219,7 @@
     <t>FMOD edits needed</t>
   </si>
   <si>
-    <t>Voice Recording</t>
-  </si>
-  <si>
     <t>KEY</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Voice Recording</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - script/voice work needed</t>
-    </r>
   </si>
   <si>
     <r>
@@ -350,6 +324,29 @@
   </si>
   <si>
     <t>Reaper Done</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(DONE) Voice Recording</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - script/voice work needed</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -511,7 +508,7 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1">
       <alignment horizontal="center"/>
@@ -526,17 +523,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="7" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="6" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="2" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="2" xfId="8" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="5" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="4" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="5" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="6" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="8" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="5" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="40% - Accent1" xfId="4" builtinId="31"/>
@@ -828,7 +824,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -917,8 +913,8 @@
       <c r="E4" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="16" t="s">
-        <v>74</v>
+      <c r="F4" s="9" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -957,8 +953,8 @@
       <c r="E6" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="F6" s="9" t="s">
-        <v>72</v>
+      <c r="F6" s="8" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -977,8 +973,8 @@
       <c r="E7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="9" t="s">
-        <v>73</v>
+      <c r="F7" s="8" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -997,7 +993,7 @@
       <c r="E8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="6" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1017,7 +1013,7 @@
       <c r="E9" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="6" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1037,7 +1033,7 @@
       <c r="E10" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="F10" s="7" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1057,8 +1053,8 @@
       <c r="E11" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F11" s="6" t="s">
-        <v>64</v>
+      <c r="F11" s="9" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1077,8 +1073,8 @@
       <c r="E12" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="F12" s="9" t="s">
-        <v>72</v>
+      <c r="F12" s="8" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1103,19 +1099,19 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D16" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D17" s="10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D18" s="11" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="E18" s="11"/>
       <c r="F18" s="11"/>
@@ -1125,28 +1121,28 @@
         <v>41</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E19" s="12"/>
       <c r="F19" s="12"/>
     </row>
     <row r="20" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D20" s="13" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E20" s="13"/>
       <c r="F20" s="13"/>
     </row>
     <row r="21" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D21" s="15" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E21" s="15"/>
       <c r="F21" s="15"/>
     </row>
     <row r="22" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D22" s="14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E22" s="14"/>
       <c r="F22" s="14"/>

</xml_diff>

<commit_message>
More sound and FMOD work
</commit_message>
<xml_diff>
--- a/DOCUMENTATION/Sound Asset List.xlsx
+++ b/DOCUMENTATION/Sound Asset List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity\Unity Projects\SpacemanLandF\DOCUMENTATION\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCCDD3DC-36EB-48B6-8591-3C2B89A40442}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A067E30A-956C-41BC-8DBD-810D7521AF42}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="73">
   <si>
     <t>Dialog</t>
   </si>
@@ -49,9 +49,6 @@
   </si>
   <si>
     <t>Player enters the main game/leaves initial main screen</t>
-  </si>
-  <si>
-    <t>Recording</t>
   </si>
   <si>
     <t>Voiceover (robotized)</t>
@@ -508,7 +505,7 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1">
       <alignment horizontal="center"/>
@@ -524,7 +521,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="7" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="6" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="2" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="2" xfId="8" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="5" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -839,7 +835,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -859,47 +855,47 @@
     </row>
     <row r="2" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" t="s">
         <v>28</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>29</v>
       </c>
-      <c r="D3" t="s">
-        <v>30</v>
-      </c>
       <c r="E3" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -911,241 +907,241 @@
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>72</v>
+        <v>8</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="F5" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
         <v>16</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>17</v>
       </c>
-      <c r="D6" t="s">
-        <v>18</v>
-      </c>
       <c r="E6" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>70</v>
+        <v>61</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>71</v>
+      <c r="F7" s="7" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
         <v>26</v>
       </c>
-      <c r="C9" t="s">
-        <v>27</v>
-      </c>
       <c r="D9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>8</v>
+        <v>36</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" t="s">
         <v>32</v>
       </c>
-      <c r="C11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" t="s">
-        <v>33</v>
-      </c>
       <c r="E11" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>72</v>
+        <v>38</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>70</v>
+        <v>44</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" t="s">
         <v>56</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>57</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>58</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="F13" s="5" t="s">
         <v>60</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D16" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D17" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
+      <c r="D17" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D18" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
+      <c r="D18" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
     </row>
     <row r="19" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C19" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D19" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+    </row>
+    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D20" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-    </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D20" s="13" t="s">
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+    </row>
+    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D21" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+    </row>
+    <row r="22" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D22" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-    </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D21" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-    </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D22" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Reaper, FMOD, Ambience Updates
Minor Reaper work for MainMenu Ambience sounds. FMOD work for MainMenuAmbience. Unity implementation of MainMenuAmbience in main menu scene.
</commit_message>
<xml_diff>
--- a/DOCUMENTATION/Sound Asset List.xlsx
+++ b/DOCUMENTATION/Sound Asset List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity\Unity Projects\SpacemanLandF\DOCUMENTATION\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{337D5D18-0B77-4A2C-ADC6-CA07A0D56632}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89B5B17E-AE6D-4577-9B30-70C1B15A38A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="77">
   <si>
     <t>Dialog</t>
   </si>
@@ -347,6 +347,15 @@
       </rPr>
       <t xml:space="preserve"> - no more edits needed in Reaper, FMOD has better options</t>
     </r>
+  </si>
+  <si>
+    <t>paramaterized timer system</t>
+  </si>
+  <si>
+    <t>paramaterized ship speed/velocity</t>
+  </si>
+  <si>
+    <t>add beeps for the ship in the space ambience</t>
   </si>
 </sst>
 </file>
@@ -578,11 +587,6 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="7" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="6" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="2" xfId="8" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="4" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="5" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="6" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="2" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -592,15 +596,20 @@
     <xf numFmtId="11" fontId="8" fillId="10" borderId="3" xfId="9" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="5" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="6" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="2" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="40% - Accent1" xfId="4" builtinId="31"/>
@@ -892,8 +901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1162,80 +1171,89 @@
       <c r="E13" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F13" s="12" t="s">
+      <c r="F13" s="7" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="9" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E16" s="17" t="s">
+      <c r="E16" s="10" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D17" s="15" t="s">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D17" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-    </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D18" s="7" t="s">
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D18" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-    </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C19" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-    </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D20" s="13"/>
-      <c r="E20" s="13" t="s">
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D20" s="8"/>
+      <c r="E20" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="F20" s="13"/>
-    </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D21" s="9" t="s">
+      <c r="F20" s="8"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>74</v>
+      </c>
+      <c r="D21" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-    </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D22" s="8" t="s">
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>75</v>
+      </c>
+      <c r="D22" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-    </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D23" s="11" t="s">
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>76</v>
+      </c>
+      <c r="D23" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="D23:F23"/>
     <mergeCell ref="D17:F17"/>
     <mergeCell ref="D18:F18"/>
     <mergeCell ref="D22:F22"/>
     <mergeCell ref="D21:F21"/>
     <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D23:F23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
All sounds done except for 2
Only things left are DialogIntro and ShipSideways. Everything else is implemented. Will change according to critique on Tuesday.
</commit_message>
<xml_diff>
--- a/DOCUMENTATION/Sound Asset List.xlsx
+++ b/DOCUMENTATION/Sound Asset List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity\Unity Projects\SpacemanLandF\DOCUMENTATION\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89B5B17E-AE6D-4577-9B30-70C1B15A38A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECBE8C2D-E7B3-4290-82F0-9FBB76ECCB52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="76">
   <si>
     <t>Dialog</t>
   </si>
@@ -202,9 +202,6 @@
   </si>
   <si>
     <t>More space movie sounds, hollow, slightly different from main menu sounds</t>
-  </si>
-  <si>
-    <t>Sounds Found</t>
   </si>
   <si>
     <t>A pinging sound. Like a submarine but with less echo. Futuristic buzzing</t>
@@ -355,14 +352,35 @@
     <t>paramaterized ship speed/velocity</t>
   </si>
   <si>
-    <t>add beeps for the ship in the space ambience</t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(DONE)</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> add beeps for the ship in the space ambience</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -440,8 +458,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -499,8 +532,20 @@
         <fgColor rgb="FFF2F2F2"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -558,8 +603,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="10">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="11" fontId="1" fillId="2" borderId="1">
       <alignment horizontal="center"/>
@@ -572,8 +630,9 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1">
       <alignment horizontal="center"/>
@@ -584,12 +643,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="7" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="6" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="2" xfId="8" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="11" fontId="1" fillId="2" borderId="1" xfId="1">
       <alignment horizontal="center"/>
     </xf>
@@ -599,6 +654,7 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="2" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -609,13 +665,19 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="4" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="5" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="6" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="2" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="5" xfId="8" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="2" xfId="10" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="10">
+  <cellStyles count="11">
     <cellStyle name="40% - Accent1" xfId="4" builtinId="31"/>
     <cellStyle name="40% - Accent2" xfId="5" builtinId="35"/>
     <cellStyle name="40% - Accent3" xfId="6" builtinId="39"/>
     <cellStyle name="40% - Accent4" xfId="7" builtinId="43"/>
+    <cellStyle name="60% - Accent3" xfId="10" builtinId="40"/>
     <cellStyle name="60% - Accent6" xfId="8" builtinId="52"/>
     <cellStyle name="Calculation" xfId="9" builtinId="22"/>
     <cellStyle name="Dark" xfId="1" xr:uid="{89477758-DE46-42CD-917F-683F060F1935}"/>
@@ -901,7 +963,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
@@ -951,8 +1013,8 @@
       <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>59</v>
+      <c r="F2" s="5" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -971,8 +1033,8 @@
       <c r="E3" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>65</v>
+      <c r="F3" s="5" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -991,8 +1053,8 @@
       <c r="E4" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>61</v>
+      <c r="F4" s="4" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1011,8 +1073,8 @@
       <c r="E5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>59</v>
+      <c r="F5" s="5" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1029,10 +1091,10 @@
         <v>17</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>65</v>
+        <v>59</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1051,8 +1113,8 @@
       <c r="E7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="6" t="s">
-        <v>65</v>
+      <c r="F7" s="5" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1071,8 +1133,8 @@
       <c r="E8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="6" t="s">
-        <v>65</v>
+      <c r="F8" s="5" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1091,8 +1153,8 @@
       <c r="E9" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F9" s="5" t="s">
-        <v>61</v>
+      <c r="F9" s="4" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1112,7 +1174,7 @@
         <v>36</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
@@ -1132,12 +1194,12 @@
         <v>38</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B12" t="s">
         <v>39</v>
@@ -1151,100 +1213,100 @@
       <c r="E12" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F12" s="6" t="s">
-        <v>65</v>
+      <c r="F12" s="17" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="F13" s="7" t="s">
-        <v>67</v>
+      <c r="F13" s="16" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C15" s="9" t="s">
-        <v>69</v>
+      <c r="C15" s="7" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D17" s="10" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D17" s="11" t="s">
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D18" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D18" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C19" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
+      <c r="D19" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D20" s="8"/>
-      <c r="E20" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="F20" s="8"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F20" s="6"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>74</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
+        <v>73</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
+        <v>74</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="D22" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>76</v>
-      </c>
-      <c r="D23" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
+      <c r="D23" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Rough Draft game sounds MS4
All sounds implemented in Unity. Will be fixed with volumes/groups/mixes etcetera in next and final milestones
</commit_message>
<xml_diff>
--- a/DOCUMENTATION/Sound Asset List.xlsx
+++ b/DOCUMENTATION/Sound Asset List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity\Unity Projects\SpacemanLandF\DOCUMENTATION\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECBE8C2D-E7B3-4290-82F0-9FBB76ECCB52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04B98702-1915-44BB-8CBF-C95C0B24A98F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -654,6 +654,12 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="2" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="5" xfId="8" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="2" xfId="10" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="2" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -665,12 +671,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="4" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="5" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="6" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="2" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="5" xfId="8" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="2" xfId="10" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="40% - Accent1" xfId="4" builtinId="31"/>
@@ -964,7 +964,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1053,8 +1053,8 @@
       <c r="E4" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>60</v>
+      <c r="F4" s="5" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1213,27 +1213,27 @@
       <c r="E12" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F12" s="17" t="s">
+      <c r="F12" s="10" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="D13" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="F13" s="9" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1248,28 +1248,28 @@
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D17" s="10" t="s">
+      <c r="D17" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C19" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="15" t="s">
+      <c r="D19" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D20" s="6"/>
@@ -1282,31 +1282,31 @@
       <c r="B21" t="s">
         <v>73</v>
       </c>
-      <c r="D21" s="14" t="s">
+      <c r="D21" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>74</v>
       </c>
-      <c r="D22" s="13" t="s">
+      <c r="D22" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="19" t="s">
+      <c r="B23" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="D23" s="9" t="s">
+      <c r="D23" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>